<commit_message>
2020.08.13_Záró km kezelés javítása út törlésekor
</commit_message>
<xml_diff>
--- a/2020-07_Tőke_Tamás_PRB-374_gkelsz.xlsx
+++ b/2020-07_Tőke_Tamás_PRB-374_gkelsz.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="93">
   <si>
     <t>ÚTNYILVÁNTARTÁS</t>
   </si>
@@ -131,7 +131,7 @@
     <t>97564</t>
   </si>
   <si>
-    <t>97936</t>
+    <t>99410</t>
   </si>
   <si>
     <t>Tőke Tamás</t>
@@ -143,10 +143,52 @@
     <t>5,7</t>
   </si>
   <si>
-    <t>20.7</t>
-  </si>
-  <si>
-    <t>2020-07-01</t>
+    <t>178.62</t>
+  </si>
+  <si>
+    <t>2020-07-06</t>
+  </si>
+  <si>
+    <t>Hibajavítás</t>
+  </si>
+  <si>
+    <t>Székesfehérvár Udvardi utca 1/A</t>
+  </si>
+  <si>
+    <t>Zirc Petőfi Sándor u. 2</t>
+  </si>
+  <si>
+    <t>CASH2512/K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>telephely/telephely</t>
+  </si>
+  <si>
+    <t>2020-07-08</t>
+  </si>
+  <si>
+    <t>Veszprém Ádám Iván u. 2.</t>
+  </si>
+  <si>
+    <t>S06041_ENA/ERSTE BANK HUNGARY Zrt</t>
+  </si>
+  <si>
+    <t>Siófok Fő u. 156-160.</t>
+  </si>
+  <si>
+    <t>EDHU0194/Euronet Banktechnikai Szolgáltató K</t>
+  </si>
+  <si>
+    <t>2020-07-09</t>
+  </si>
+  <si>
+    <t>telephelytelephely</t>
+  </si>
+  <si>
+    <t>2020-07-11</t>
   </si>
   <si>
     <t>Magán</t>
@@ -155,22 +197,121 @@
     <t>Magánhasználat</t>
   </si>
   <si>
-    <t>Hibajavítás</t>
-  </si>
-  <si>
-    <t>Székesfehérvár Udvardi utca 1/A</t>
-  </si>
-  <si>
-    <t>Csömör Szabadság út 16.</t>
-  </si>
-  <si>
-    <t>S6T65121MTB Magyar Takarékszövetkezeti Bank</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>telephely/telephely</t>
+    <t>2020-07-13</t>
+  </si>
+  <si>
+    <t>Tamási Szabadság út 33.</t>
+  </si>
+  <si>
+    <t>DBD82220238/OTP BANK Nyrt.</t>
+  </si>
+  <si>
+    <t>2020-07-14</t>
+  </si>
+  <si>
+    <t>Székesfehérvár Kossuth u. 14.</t>
+  </si>
+  <si>
+    <t>MGND2401/MagNet Magyar Közösségi Bank Zrt.</t>
+  </si>
+  <si>
+    <t>2020-07-15</t>
+  </si>
+  <si>
+    <t>Veszprém Szabadság tér 8.</t>
+  </si>
+  <si>
+    <t>S6T17614/Sopron Bank Zrt.</t>
+  </si>
+  <si>
+    <t>2020-07-16</t>
+  </si>
+  <si>
+    <t>Mór Deák F. u. 2.</t>
+  </si>
+  <si>
+    <t>DBD82220135/OTP BANK Nyrt.</t>
+  </si>
+  <si>
+    <t>2020-07-17</t>
+  </si>
+  <si>
+    <t>Balatonboglár Dózsa Gy. u. 1.</t>
+  </si>
+  <si>
+    <t>DBD82220236OTP BANK Nyrt.</t>
+  </si>
+  <si>
+    <t>2020-07-20</t>
+  </si>
+  <si>
+    <t>Öttevény Fő út 104</t>
+  </si>
+  <si>
+    <t>S6T59005/MTB Magyar Takarékszövetkezeti Bank</t>
+  </si>
+  <si>
+    <t>2020-07-21</t>
+  </si>
+  <si>
+    <t>Veszprém Ady Endre u. 1.</t>
+  </si>
+  <si>
+    <t>CA38_ENA/UniCredit Bank Hungary Zrt.</t>
+  </si>
+  <si>
+    <t>2020-07-22</t>
+  </si>
+  <si>
+    <t>Székesfehérvár Balatoni u. 21.</t>
+  </si>
+  <si>
+    <t>CIB - ATM638/CIB Bank Zrt</t>
+  </si>
+  <si>
+    <t>2020-07-24</t>
+  </si>
+  <si>
+    <t>Ajka Szabadság tér 18.</t>
+  </si>
+  <si>
+    <t>DBD82220092/OTP BANK Nyrt.</t>
+  </si>
+  <si>
+    <t>2020-07-27</t>
+  </si>
+  <si>
+    <t>Siófok Fő tér 1.</t>
+  </si>
+  <si>
+    <t>S09210ERSTE BANK HUNGARY Zrt</t>
+  </si>
+  <si>
+    <t>2020-07-28</t>
+  </si>
+  <si>
+    <t>Veszprém Cserhát ltp. 8.</t>
+  </si>
+  <si>
+    <t>CASH2283K &amp; H BANK ZRT.</t>
+  </si>
+  <si>
+    <t>2020-07-30</t>
+  </si>
+  <si>
+    <t>Várpalota Újlaki u. 2.</t>
+  </si>
+  <si>
+    <t>DBD82220228OTP BANK Nyrt.</t>
+  </si>
+  <si>
+    <t>2020-07-31</t>
+  </si>
+  <si>
+    <t>Ságvár Petőfi u. 18/6</t>
+  </si>
+  <si>
+    <t>S6T50827/MTB Magyar Takarékszövetkezeti Bank</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1263,7 @@
       </c>
       <c r="G5" s="8" t="str">
         <f>SUM(I10:I105)</f>
-        <v>372</v>
+        <v>1846</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -1139,7 +1280,7 @@
       </c>
       <c r="G6" s="9" t="str">
         <f>100*G7/G5</f>
-        <v>5.564</v>
+        <v>9.676</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
@@ -1225,23 +1366,23 @@
         <v>39</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G10" s="26" t="n">
         <f>IF(B10&lt;&gt;"",$C$5+I10,"")</f>
-        <v>97675.0</v>
+        <v>97625.0</v>
       </c>
       <c r="H10" s="21" t="n">
-        <v>12.2</v>
+        <v>0.0</v>
       </c>
       <c r="I10" s="21" t="n">
-        <v>111.0</v>
+        <v>61.0</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1255,26 +1396,26 @@
         <v>38</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G11" s="26" t="n">
         <f>IF(B11&lt;&gt;"",G10+I11,"")</f>
-        <v>97786.0</v>
+        <v>97686.0</v>
       </c>
       <c r="H11" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I11" s="21" t="n">
-        <v>111.0</v>
+        <v>61.0</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1282,32 +1423,32 @@
         <v>3</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G12" s="26" t="n">
         <f t="shared" ref="G12:G54" si="0">IF(B12&lt;&gt;"",G11+I12,"")</f>
-        <v>97861.0</v>
+        <v>97735.0</v>
       </c>
       <c r="H12" s="21" t="n">
-        <v>8.5</v>
+        <v>0.0</v>
       </c>
       <c r="I12" s="21" t="n">
-        <v>75.0</v>
+        <v>49.0</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K12" s="43"/>
       <c r="L12" s="43"/>
@@ -1318,32 +1459,32 @@
         <v>4</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G13" s="26" t="n">
         <f t="shared" si="0"/>
-        <v>97936.0</v>
+        <v>97783.0</v>
       </c>
       <c r="H13" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I13" s="21" t="n">
-        <v>75.0</v>
+        <v>48.0</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K13" s="43"/>
       <c r="L13" s="43"/>
@@ -1353,511 +1494,991 @@
       <c r="A14" s="19">
         <v>5</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="19"/>
+      <c r="B14" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>97837.0</v>
+      </c>
+      <c r="H14" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="21" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>6</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="19"/>
+      <c r="B15" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>97891.0</v>
+      </c>
+      <c r="H15" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" s="21" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>7</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="19"/>
+      <c r="B16" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>97945.0</v>
+      </c>
+      <c r="H16" s="21" t="n">
+        <v>47.53</v>
+      </c>
+      <c r="I16" s="21" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>8</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="19"/>
+      <c r="B17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98000.0</v>
+      </c>
+      <c r="H17" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="21" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>9</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="19"/>
+      <c r="B18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98090.0</v>
+      </c>
+      <c r="H18" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I18" s="21" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>10</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="19"/>
+      <c r="B19" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98180.0</v>
+      </c>
+      <c r="H19" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I19" s="21" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>12</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="19"/>
+      <c r="B20" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98185.0</v>
+      </c>
+      <c r="H20" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I20" s="21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>13</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="19"/>
+      <c r="B21" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98190.0</v>
+      </c>
+      <c r="H21" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I21" s="21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>14</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="19"/>
+      <c r="B22" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98239.0</v>
+      </c>
+      <c r="H22" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I22" s="21" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>15</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="19"/>
+      <c r="B23" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98288.0</v>
+      </c>
+      <c r="H23" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I23" s="21" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>16</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="19"/>
+      <c r="B24" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98318.0</v>
+      </c>
+      <c r="H24" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I24" s="21" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>17</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="19"/>
+      <c r="B25" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98348.0</v>
+      </c>
+      <c r="H25" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I25" s="21" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>19</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="19"/>
+      <c r="B26" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98440.0</v>
+      </c>
+      <c r="H26" s="21" t="n">
+        <v>45.75</v>
+      </c>
+      <c r="I26" s="21" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>20</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="19"/>
+      <c r="B27" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98532.0</v>
+      </c>
+      <c r="H27" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I27" s="21" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>21</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98637.0</v>
+      </c>
+      <c r="H28" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I28" s="21" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>22</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98742.0</v>
+      </c>
+      <c r="H29" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I29" s="21" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>23</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="19"/>
+      <c r="B30" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98791.0</v>
+      </c>
+      <c r="H30" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I30" s="21" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>24</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="19"/>
+      <c r="B31" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98840.0</v>
+      </c>
+      <c r="H31" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I31" s="21" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>25</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="19"/>
+      <c r="B32" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98846.0</v>
+      </c>
+      <c r="H32" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I32" s="21" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>26</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="19"/>
+      <c r="B33" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98852.0</v>
+      </c>
+      <c r="H33" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I33" s="21" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>29</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="19"/>
+      <c r="B34" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>98934.0</v>
+      </c>
+      <c r="H34" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I34" s="21" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="24">
         <v>30</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="19"/>
+      <c r="B35" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99016.0</v>
+      </c>
+      <c r="H35" s="21" t="n">
+        <v>46.48</v>
+      </c>
+      <c r="I35" s="21" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>31</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="19"/>
+      <c r="B36" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99070.0</v>
+      </c>
+      <c r="H36" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I36" s="21" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>32</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="19"/>
+      <c r="B37" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99124.0</v>
+      </c>
+      <c r="H37" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I37" s="21" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>33</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="19"/>
+      <c r="B38" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99174.0</v>
+      </c>
+      <c r="H38" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I38" s="21" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>34</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="19"/>
+      <c r="B39" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99224.0</v>
+      </c>
+      <c r="H39" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I39" s="21" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>35</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="19"/>
+      <c r="B40" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99256.0</v>
+      </c>
+      <c r="H40" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I40" s="21" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>36</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="19"/>
+      <c r="B41" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99288.0</v>
+      </c>
+      <c r="H41" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I41" s="21" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>37</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="19"/>
+      <c r="B42" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99349.0</v>
+      </c>
+      <c r="H42" s="21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I42" s="21" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>38</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="19"/>
+      <c r="B43" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="26" t="n">
+        <f t="shared" si="0"/>
+        <v>99410.0</v>
+      </c>
+      <c r="H43" s="21" t="n">
+        <v>38.86</v>
+      </c>
+      <c r="I43" s="21" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="19">
@@ -2883,7 +3504,7 @@
       </c>
       <c r="L103" s="35" t="str">
         <f>SUM(I10:I105)</f>
-        <v>372</v>
+        <v>1846</v>
       </c>
       <c r="M103" s="36"/>
     </row>
@@ -2908,11 +3529,11 @@
       </c>
       <c r="L104" s="38" t="str">
         <f>SUMIF(J10:J105,"M",I10:I105)</f>
-        <v>222</v>
+        <v>55</v>
       </c>
       <c r="M104" s="39" t="str">
         <f>L104/L103</f>
-        <v>59%</v>
+        <v>2.%</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -2936,7 +3557,7 @@
       </c>
       <c r="L105" s="41" t="str">
         <f>C5+L103</f>
-        <v>97936</v>
+        <v>99410</v>
       </c>
       <c r="M105" s="42"/>
     </row>

</xml_diff>